<commit_message>
Fixed issue with HTML entities, such as &pound; being referenced, but not declared
</commit_message>
<xml_diff>
--- a/src/test/resources/org/concordion/ext/excel/CellConversions.xlsx
+++ b/src/test/resources/org/concordion/ext/excel/CellConversions.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6940" yWindow="3660" windowWidth="24960" windowHeight="15060" tabRatio="500"/>
+    <workbookView xWindow="6945" yWindow="3660" windowWidth="20730" windowHeight="12180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +24,7 @@
     <author>Rob Moffat</author>
   </authors>
   <commentList>
-    <comment ref="A8" authorId="0">
+    <comment ref="A10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Number Examples</t>
   </si>
@@ -71,16 +71,28 @@
   </si>
   <si>
     <t>Check the formatting</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>&lt; &amp; &gt; ' "</t>
+  </si>
+  <si>
+    <t>Text with XML entities</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
     <numFmt numFmtId="165" formatCode="[$-809]dd\ mmmm\ yyyy;@"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="168" formatCode="[$£-809]#,##0.00"/>
+    <numFmt numFmtId="169" formatCode="[$฿-41E]#,##0.00"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -142,7 +154,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -151,6 +163,9 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -159,6 +174,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -484,18 +504,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:G8"/>
+  <dimension ref="A3:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -512,7 +532,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -532,7 +552,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -549,7 +569,7 @@
         <v>AB</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -560,15 +580,39 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="8">
+        <v>6.7889999999999997</v>
+      </c>
+      <c r="D7" s="9">
+        <v>50</v>
+      </c>
+      <c r="E7" s="10">
+        <v>1234.56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="10"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Removed checks of &quot; and &apos; from 2d6aa04d24e45504b4062db8366e6bc8a81b4f05 since these are treated differently between Java 7 and 8
</commit_message>
<xml_diff>
--- a/src/test/resources/org/concordion/ext/excel/CellConversions.xlsx
+++ b/src/test/resources/org/concordion/ext/excel/CellConversions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6945" yWindow="3660" windowWidth="20730" windowHeight="12180" tabRatio="500"/>
+    <workbookView xWindow="6945" yWindow="3660" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -76,10 +76,10 @@
     <t>Currency</t>
   </si>
   <si>
-    <t>&lt; &amp; &gt; ' "</t>
-  </si>
-  <si>
     <t>Text with XML entities</t>
+  </si>
+  <si>
+    <t>&lt; &amp; &gt;</t>
   </si>
 </sst>
 </file>
@@ -507,7 +507,7 @@
   <dimension ref="A3:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -596,10 +596,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>8</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>7</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="10"/>

</xml_diff>